<commit_message>
Updated workbook with excel functionalities
</commit_message>
<xml_diff>
--- a/Data_Cleaning/data/sample_excel_output.xlsx
+++ b/Data_Cleaning/data/sample_excel_output.xlsx
@@ -1,50 +1,87 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27126"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\wengz\Desktop\ZS_Github\Data_Engineering\Data_Cleaning\data\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6308CB16-FA8F-498F-AF3C-B9B32ECB0BD0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="600" firstSheet="0" activeTab="1" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="hidden" sheetId="1" r:id="rId1"/>
-    <sheet name="formatted" sheetId="2" r:id="rId2"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="hidden" sheetId="1" state="hidden" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="formatted" sheetId="2" state="visible" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="162913"/>
-  <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
-      <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-  </extLst>
+  <definedNames/>
+  <calcPr calcId="191029" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="0"/>
+  <fonts count="4">
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <color theme="1"/>
+      <sz val="11"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <b val="1"/>
+      <sz val="11"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <b val="1"/>
+      <color theme="0"/>
+      <sz val="11"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b val="1"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="7">
     <fill>
-      <patternFill patternType="none"/>
+      <patternFill/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B0F0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF7030A0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -52,26 +89,118 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+  <cellXfs count="9">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="1" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="1" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008000"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00808000"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="00C0C0C0"/>
+      <rgbColor rgb="00808080"/>
+      <rgbColor rgb="009999FF"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00FFFFCC"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00660066"/>
+      <rgbColor rgb="00FF8080"/>
+      <rgbColor rgb="000066CC"/>
+      <rgbColor rgb="00CCCCFF"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="0000CCFF"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00CCFFCC"/>
+      <rgbColor rgb="00FFFF99"/>
+      <rgbColor rgb="0099CCFF"/>
+      <rgbColor rgb="00FF99CC"/>
+      <rgbColor rgb="00CC99FF"/>
+      <rgbColor rgb="00FFCC99"/>
+      <rgbColor rgb="003366FF"/>
+      <rgbColor rgb="0033CCCC"/>
+      <rgbColor rgb="0099CC00"/>
+      <rgbColor rgb="00FFCC00"/>
+      <rgbColor rgb="00FF9900"/>
+      <rgbColor rgb="00FF6600"/>
+      <rgbColor rgb="00666699"/>
+      <rgbColor rgb="00969696"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
+    </indexedColors>
+  </colors>
 </styleSheet>
 </file>
 
@@ -337,25 +466,394 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:G6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="8" t="inlineStr">
+        <is>
+          <t>Field</t>
+        </is>
+      </c>
+      <c r="B1" s="8" t="inlineStr">
+        <is>
+          <t>Field Name</t>
+        </is>
+      </c>
+      <c r="C1" s="8" t="inlineStr">
+        <is>
+          <t>Data element</t>
+        </is>
+      </c>
+      <c r="D1" s="8" t="inlineStr">
+        <is>
+          <t>Checktable</t>
+        </is>
+      </c>
+      <c r="E1" s="8" t="inlineStr">
+        <is>
+          <t>Datatype</t>
+        </is>
+      </c>
+      <c r="F1" s="8" t="inlineStr">
+        <is>
+          <t>Length</t>
+        </is>
+      </c>
+      <c r="G1" s="8" t="inlineStr">
+        <is>
+          <t>Decimals</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>MANDT</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>Client</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>MANDT</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>T000</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>CLNT</t>
+        </is>
+      </c>
+      <c r="F2" t="n">
+        <v>3</v>
+      </c>
+      <c r="G2" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>MATNR</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>Material Number</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>MATNR</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>MARA</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>CHAR</t>
+        </is>
+      </c>
+      <c r="F3" t="n">
+        <v>18</v>
+      </c>
+      <c r="G3" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>SPRAS</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>Language Key</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>SPRAS</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>T002</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>LANG</t>
+        </is>
+      </c>
+      <c r="F4" t="n">
+        <v>1</v>
+      </c>
+      <c r="G4" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>MAKTX</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>Material Description (Short Text)</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>MAKTX</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>CHAR</t>
+        </is>
+      </c>
+      <c r="F5" t="n">
+        <v>40</v>
+      </c>
+      <c r="G5" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>MAKTG</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>Material description in upper case for matchcodes</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>MAKTG</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>CHAR</t>
+        </is>
+      </c>
+      <c r="F6" t="n">
+        <v>40</v>
+      </c>
+      <c r="G6" t="n">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6A219E51-0CE4-439D-830E-2A6F49E28E11}">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:F6"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G12" sqref="G12"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <cols>
+    <col width="7.7109375" bestFit="1" customWidth="1" min="1" max="1"/>
+    <col width="46.28515625" bestFit="1" customWidth="1" min="2" max="2"/>
+    <col width="13.140625" bestFit="1" customWidth="1" min="3" max="3"/>
+    <col width="10.85546875" bestFit="1" customWidth="1" min="4" max="4"/>
+    <col width="9" bestFit="1" customWidth="1" min="5" max="5"/>
+  </cols>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="3">
+        <f>hidden!A1</f>
+        <v/>
+      </c>
+      <c r="B1" s="4">
+        <f>hidden!B1</f>
+        <v/>
+      </c>
+      <c r="C1" s="5">
+        <f>hidden!C1</f>
+        <v/>
+      </c>
+      <c r="D1" s="6">
+        <f>hidden!D1</f>
+        <v/>
+      </c>
+      <c r="E1" s="4">
+        <f>hidden!E1</f>
+        <v/>
+      </c>
+      <c r="F1" s="7">
+        <f>hidden!F1</f>
+        <v/>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="2">
+        <f>hidden!A2</f>
+        <v/>
+      </c>
+      <c r="B2" s="2">
+        <f>hidden!B2</f>
+        <v/>
+      </c>
+      <c r="C2" s="2">
+        <f>hidden!C2</f>
+        <v/>
+      </c>
+      <c r="D2" s="2">
+        <f>hidden!D2</f>
+        <v/>
+      </c>
+      <c r="E2" s="2">
+        <f>hidden!E2</f>
+        <v/>
+      </c>
+      <c r="F2" s="2">
+        <f>hidden!F2</f>
+        <v/>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="2">
+        <f>hidden!A3</f>
+        <v/>
+      </c>
+      <c r="B3" s="2">
+        <f>hidden!B3</f>
+        <v/>
+      </c>
+      <c r="C3" s="2">
+        <f>hidden!C3</f>
+        <v/>
+      </c>
+      <c r="D3" s="2">
+        <f>hidden!D3</f>
+        <v/>
+      </c>
+      <c r="E3" s="2">
+        <f>hidden!E3</f>
+        <v/>
+      </c>
+      <c r="F3" s="2">
+        <f>hidden!F3</f>
+        <v/>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="2">
+        <f>hidden!A4</f>
+        <v/>
+      </c>
+      <c r="B4" s="2">
+        <f>hidden!B4</f>
+        <v/>
+      </c>
+      <c r="C4" s="2">
+        <f>hidden!C4</f>
+        <v/>
+      </c>
+      <c r="D4" s="2">
+        <f>hidden!D4</f>
+        <v/>
+      </c>
+      <c r="E4" s="2">
+        <f>hidden!E4</f>
+        <v/>
+      </c>
+      <c r="F4" s="2">
+        <f>hidden!F4</f>
+        <v/>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="2">
+        <f>hidden!A5</f>
+        <v/>
+      </c>
+      <c r="B5" s="2">
+        <f>hidden!B5</f>
+        <v/>
+      </c>
+      <c r="C5" s="2">
+        <f>hidden!C5</f>
+        <v/>
+      </c>
+      <c r="D5" s="2">
+        <f>hidden!D5</f>
+        <v/>
+      </c>
+      <c r="E5" s="2">
+        <f>hidden!E5</f>
+        <v/>
+      </c>
+      <c r="F5" s="2">
+        <f>hidden!F5</f>
+        <v/>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="2">
+        <f>hidden!A6</f>
+        <v/>
+      </c>
+      <c r="B6" s="2">
+        <f>hidden!B6</f>
+        <v/>
+      </c>
+      <c r="C6" s="2">
+        <f>hidden!C6</f>
+        <v/>
+      </c>
+      <c r="D6" s="2">
+        <f>hidden!D6</f>
+        <v/>
+      </c>
+      <c r="E6" s="2">
+        <f>hidden!E6</f>
+        <v/>
+      </c>
+      <c r="F6" s="2">
+        <f>hidden!F6</f>
+        <v/>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>